<commit_message>
Read xmlx sheet entries to set
</commit_message>
<xml_diff>
--- a/dict.xlsx
+++ b/dict.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B3EAD-08F8-4692-AED2-4BF409255ADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4E6252-CE30-4C8A-B2EC-E3352251B75B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="900" windowWidth="21150" windowHeight="15300" xr2:uid="{1088CA62-C64D-4A4C-8383-8DE6664B7634}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1088CA62-C64D-4A4C-8383-8DE6664B7634}"/>
   </bookViews>
   <sheets>
     <sheet name="Eng_dict" sheetId="1" r:id="rId1"/>
     <sheet name="Germ_dict" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Eng_dict!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Eng_dict!$A$1:$K$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1862,7 +1862,7 @@
   <dimension ref="B3:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K28"/>
+      <selection sqref="A1:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,8 +2568,9 @@
       </c>
     </row>
   </sheetData>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="2" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="2" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>